<commit_message>
Added some error handling, added new AITS program to script
</commit_message>
<xml_diff>
--- a/Output Files/KC 2025-26 Applications KPI as of June 02, 2025.xlsx
+++ b/Output Files/KC 2025-26 Applications KPI as of June 02, 2025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -1635,7 +1635,70 @@
     <cellStyle name="Normal 5" xfId="8"/>
     <cellStyle name="Normal 6" xfId="9"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2831,7 +2894,7 @@
         <v>1425</v>
       </c>
       <c r="I12" s="50" t="n">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="J12" s="49" t="n">
         <v>39</v>
@@ -2840,10 +2903,10 @@
         <v>39</v>
       </c>
       <c r="L12" s="49" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="M12" s="51" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="50.1" customHeight="1" s="53">
@@ -2955,37 +3018,37 @@
     </row>
     <row r="18" ht="15.75" customHeight="1" s="53">
       <c r="E18" s="46" t="n">
-        <v>1406</v>
+        <v>1297</v>
       </c>
       <c r="F18" s="47" t="n">
-        <v>1611</v>
+        <v>1297</v>
       </c>
       <c r="G18" s="48" t="n">
-        <v>537</v>
+        <v>469</v>
       </c>
       <c r="H18" s="49" t="n">
-        <v>4708</v>
+        <v>4369</v>
       </c>
       <c r="I18" s="50" t="n">
-        <v>5084</v>
+        <v>4655</v>
       </c>
       <c r="J18" s="49" t="n">
-        <v>3046</v>
+        <v>2479</v>
       </c>
       <c r="K18" s="52" t="n">
-        <v>3382</v>
+        <v>2713</v>
       </c>
       <c r="L18" s="49" t="n">
-        <v>2097</v>
+        <v>1645</v>
       </c>
       <c r="M18" s="51" t="n">
-        <v>2282</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="19" ht="50.1" customHeight="1" s="53" thickBot="1">
       <c r="E19" s="182" t="inlineStr">
         <is>
-          <t>*The unique number of 1406 Fall Applicants is 70.1% lower in comparison with Fall 2024. The number of International applications is 493 representing 30.6% of total applications.</t>
+          <t>*The unique number of 1297 Fall Applicants is 70.3% lower in comparison with Fall 2024. The number of International applications is 441 representing 34.0% of total applications.</t>
         </is>
       </c>
       <c r="F19" s="183" t="n"/>
@@ -3093,37 +3156,37 @@
     </row>
     <row r="24" ht="15.75" customHeight="1" s="53">
       <c r="E24" s="46" t="n">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="F24" s="47" t="n">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="G24" s="48" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H24" s="49" t="n">
-        <v>1125</v>
+        <v>994</v>
       </c>
       <c r="I24" s="50" t="n">
-        <v>1146</v>
+        <v>1007</v>
       </c>
       <c r="J24" s="49" t="n">
-        <v>1446</v>
+        <v>326</v>
       </c>
       <c r="K24" s="50" t="n">
-        <v>1462</v>
+        <v>331</v>
       </c>
       <c r="L24" s="49" t="n">
-        <v>302</v>
+        <v>115</v>
       </c>
       <c r="M24" s="51" t="n">
-        <v>305</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" ht="50.1" customHeight="1" s="53" thickBot="1">
       <c r="E25" s="182" t="inlineStr">
         <is>
-          <t>*The unique number of 110 Winter Applicants is 90.2% lower in comparison with Winter 2025. The number of International applications is 68 representing 57.6% of total applications.</t>
+          <t>*The unique number of 33 Winter Applicants is 96.7% lower in comparison with Winter 2025. The number of International applications is 21 representing 63.6% of total applications.</t>
         </is>
       </c>
       <c r="F25" s="183" t="n"/>
@@ -3230,10 +3293,10 @@
     <row r="30" ht="15.75" customHeight="1" s="53">
       <c r="C30" s="57" t="n"/>
       <c r="E30" s="46" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F30" s="47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30" s="48" t="n">
         <v>0</v>
@@ -3245,22 +3308,22 @@
         <v>2</v>
       </c>
       <c r="J30" s="49" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="K30" s="50" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="L30" s="49" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="M30" s="51" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" ht="50.1" customHeight="1" s="53">
       <c r="E31" s="180" t="inlineStr">
         <is>
-          <t>*The unique number of 2 Spring Applicants is 0.0% higher in comparison with Spring 2025. The number of International applications is 0 representing 0.0% of total applications.</t>
+          <t>*The unique number of 1 Spring Applicants is 50.0% lower in comparison with Spring 2025. The number of International applications is 0 representing 0.0% of total applications.</t>
         </is>
       </c>
       <c r="F31" s="165" t="n"/>
@@ -3314,9 +3377,9 @@
   </sheetPr>
   <dimension ref="A1:P195"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A194" sqref="A194"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P120" sqref="P120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3696,10 +3759,10 @@
       </c>
       <c r="G10" s="161" t="n"/>
       <c r="H10" s="9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I10" s="35" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J10" s="9" t="n"/>
       <c r="K10" s="35" t="n"/>
@@ -3707,10 +3770,10 @@
       <c r="M10" s="35" t="n"/>
       <c r="N10" s="35" t="n"/>
       <c r="O10" s="35" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="53">
@@ -3764,10 +3827,10 @@
       </c>
       <c r="G12" s="195" t="n"/>
       <c r="H12" s="9" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I12" s="35" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J12" s="9" t="n"/>
       <c r="K12" s="35" t="n"/>
@@ -3775,7 +3838,7 @@
       <c r="M12" s="35" t="n"/>
       <c r="N12" s="35" t="n"/>
       <c r="O12" s="35" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P12" s="3" t="n">
         <v>1</v>
@@ -7111,7 +7174,11 @@
           <t>Applied IT Specialist</t>
         </is>
       </c>
-      <c r="D119" s="25" t="n"/>
+      <c r="D119" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>Domestic</t>
@@ -7139,7 +7206,11 @@
       <c r="A120" s="192" t="n"/>
       <c r="B120" s="193" t="n"/>
       <c r="C120" s="161" t="n"/>
-      <c r="D120" s="25" t="n"/>
+      <c r="D120" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E120" s="2" t="inlineStr">
         <is>
           <t>International</t>
@@ -8979,10 +9050,10 @@
       <c r="M176" s="35" t="n"/>
       <c r="N176" s="35" t="n"/>
       <c r="O176" s="35" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P176" s="3" t="n">
-        <v>0.8421052631578947</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="177" ht="15.75" customHeight="1" s="53">
@@ -9431,10 +9502,10 @@
         <v>0</v>
       </c>
       <c r="O190" s="4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P190" s="39" t="n">
-        <v>0.8695652173913043</v>
+        <v>0.9130434782608695</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" s="53">
@@ -9471,10 +9542,10 @@
         <v>0</v>
       </c>
       <c r="O191" s="5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P191" s="40" t="n">
-        <v>0.8695652173913043</v>
+        <v>0.9130434782608695</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" s="53">
@@ -9511,10 +9582,10 @@
         <v>0</v>
       </c>
       <c r="O192" s="8" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P192" s="12" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" s="53">
@@ -9767,7 +9838,29 @@
     <mergeCell ref="C147:C148"/>
     <mergeCell ref="G145:G146"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I120 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I118 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="2">
+      <formula>10</formula>
+      <formula>100000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="1">
+      <formula>1</formula>
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8" dxfId="0">
+      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P118 P121:P1048576">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I119:I120">
     <cfRule type="cellIs" priority="2" operator="between" dxfId="2">
       <formula>10</formula>
       <formula>100000000</formula>
@@ -9777,10 +9870,10 @@
       <formula>9</formula>
     </cfRule>
     <cfRule type="expression" priority="4" dxfId="0">
-      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+      <formula>AND(I119=0, I119&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P119:P120">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
@@ -9801,9 +9894,9 @@
   </sheetPr>
   <dimension ref="A1:P195"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A193" sqref="A193:P193"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P119" sqref="P119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -9959,22 +10052,20 @@
         </is>
       </c>
       <c r="H3" s="9" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I3" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="9" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J3" s="9" t="n"/>
       <c r="K3" s="35" t="n"/>
       <c r="L3" s="35" t="n"/>
       <c r="M3" s="35" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N3" s="35" t="n"/>
       <c r="O3" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P3" s="3" t="n">
         <v>1</v>
@@ -10002,19 +10093,21 @@
         <v>2</v>
       </c>
       <c r="I4" s="35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="9" t="n"/>
       <c r="K4" s="35" t="n"/>
       <c r="L4" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="M4" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M4" s="35" t="n"/>
       <c r="N4" s="35" t="n"/>
-      <c r="O4" s="35" t="n"/>
-      <c r="P4" s="3" t="n"/>
+      <c r="O4" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="53">
       <c r="A5" s="192" t="n"/>
@@ -10043,12 +10136,14 @@
         </is>
       </c>
       <c r="H5" s="9" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5" s="35" t="n">
-        <v>16</v>
-      </c>
-      <c r="J5" s="9" t="n"/>
+        <v>13</v>
+      </c>
+      <c r="J5" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K5" s="35" t="n"/>
       <c r="L5" s="35" t="n">
         <v>1</v>
@@ -10058,10 +10153,10 @@
       </c>
       <c r="N5" s="35" t="n"/>
       <c r="O5" s="35" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="P5" s="3" t="n">
-        <v>0.75</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="53">
@@ -10083,26 +10178,22 @@
       </c>
       <c r="G6" s="161" t="n"/>
       <c r="H6" s="9" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" s="35" t="n">
         <v>5</v>
       </c>
       <c r="J6" s="9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="35" t="n"/>
       <c r="L6" s="35" t="n"/>
       <c r="M6" s="35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6" s="35" t="n"/>
-      <c r="O6" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="P6" s="3" t="n">
-        <v>0.4</v>
-      </c>
+      <c r="O6" s="35" t="n"/>
+      <c r="P6" s="3" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="53">
       <c r="A7" s="192" t="n"/>
@@ -10127,10 +10218,10 @@
         </is>
       </c>
       <c r="H7" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="9" t="n"/>
       <c r="K7" s="35" t="n"/>
@@ -10138,7 +10229,7 @@
       <c r="M7" s="35" t="n"/>
       <c r="N7" s="35" t="n"/>
       <c r="O7" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7" s="3" t="n">
         <v>1</v>
@@ -10163,10 +10254,10 @@
       </c>
       <c r="G8" s="161" t="n"/>
       <c r="H8" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="9" t="n"/>
       <c r="K8" s="35" t="n"/>
@@ -10174,7 +10265,7 @@
       <c r="M8" s="35" t="n"/>
       <c r="N8" s="35" t="n"/>
       <c r="O8" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8" s="3" t="n">
         <v>1</v>
@@ -10207,27 +10298,27 @@
         </is>
       </c>
       <c r="H9" s="9" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="I9" s="35" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J9" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K9" s="35" t="n"/>
       <c r="L9" s="35" t="n">
         <v>1</v>
       </c>
       <c r="M9" s="35" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="N9" s="35" t="n"/>
       <c r="O9" s="35" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="P9" s="3" t="n">
-        <v>0.8260869565217391</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="53">
@@ -10249,27 +10340,25 @@
       </c>
       <c r="G10" s="161" t="n"/>
       <c r="H10" s="9" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I10" s="35" t="n">
-        <v>16</v>
-      </c>
-      <c r="J10" s="9" t="n">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="J10" s="9" t="n"/>
       <c r="K10" s="35" t="n"/>
       <c r="L10" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M10" s="35" t="n">
         <v>5</v>
       </c>
       <c r="N10" s="35" t="n"/>
       <c r="O10" s="35" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="P10" s="3" t="n">
-        <v>0.625</v>
+        <v>0.5909090909090909</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="53">
@@ -10323,10 +10412,10 @@
       </c>
       <c r="G12" s="195" t="n"/>
       <c r="H12" s="9" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="I12" s="35" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="J12" s="9" t="n"/>
       <c r="K12" s="35" t="n"/>
@@ -10334,10 +10423,10 @@
       <c r="M12" s="35" t="n"/>
       <c r="N12" s="35" t="n"/>
       <c r="O12" s="35" t="n">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="P12" s="3" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="53">
@@ -10503,25 +10592,23 @@
         </is>
       </c>
       <c r="H17" s="9" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I17" s="35" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J17" s="9" t="n"/>
       <c r="K17" s="35" t="n"/>
-      <c r="L17" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L17" s="35" t="n"/>
       <c r="M17" s="35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N17" s="35" t="n"/>
       <c r="O17" s="35" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P17" s="3" t="n">
-        <v>0.75</v>
+        <v>0.4285714285714285</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="53">
@@ -10543,23 +10630,23 @@
       </c>
       <c r="G18" s="193" t="n"/>
       <c r="H18" s="9" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I18" s="35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J18" s="9" t="n"/>
       <c r="K18" s="35" t="n"/>
       <c r="L18" s="35" t="n"/>
       <c r="M18" s="35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N18" s="35" t="n"/>
       <c r="O18" s="35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P18" s="3" t="n">
-        <v>0.8</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="53">
@@ -10687,27 +10774,27 @@
       </c>
       <c r="G22" s="193" t="n"/>
       <c r="H22" s="9" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I22" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="J22" s="9" t="n"/>
-      <c r="K22" s="35" t="n">
-        <v>4</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="J22" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="K22" s="35" t="n"/>
       <c r="L22" s="35" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M22" s="35" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N22" s="35" t="n"/>
       <c r="O22" s="35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P22" s="3" t="n">
-        <v>0.5</v>
+        <v>0.04761904761904762</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="53">
@@ -11055,12 +11142,8 @@
       <c r="L33" s="35" t="n"/>
       <c r="M33" s="35" t="n"/>
       <c r="N33" s="35" t="n"/>
-      <c r="O33" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P33" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O33" s="35" t="n"/>
+      <c r="P33" s="3" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="53">
       <c r="A34" s="192" t="n"/>
@@ -11313,11 +11396,11 @@
         <v>0</v>
       </c>
       <c r="J41" s="9" t="n"/>
-      <c r="K41" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="K41" s="35" t="n"/>
       <c r="L41" s="35" t="n"/>
-      <c r="M41" s="35" t="n"/>
+      <c r="M41" s="35" t="n">
+        <v>1</v>
+      </c>
       <c r="N41" s="35" t="n"/>
       <c r="O41" s="35" t="n"/>
       <c r="P41" s="3" t="n"/>
@@ -11470,17 +11553,11 @@
         <v>1</v>
       </c>
       <c r="G46" s="161" t="n"/>
-      <c r="H46" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H46" s="9" t="n"/>
+      <c r="I46" s="35" t="n"/>
       <c r="J46" s="9" t="n"/>
       <c r="K46" s="35" t="n"/>
-      <c r="L46" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L46" s="35" t="n"/>
       <c r="M46" s="35" t="n"/>
       <c r="N46" s="35" t="n"/>
       <c r="O46" s="35" t="n"/>
@@ -11573,16 +11650,16 @@
         </is>
       </c>
       <c r="H49" s="9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I49" s="35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="9" t="n"/>
       <c r="K49" s="35" t="n"/>
       <c r="L49" s="35" t="n"/>
       <c r="M49" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N49" s="35" t="n"/>
       <c r="O49" s="35" t="n"/>
@@ -11645,25 +11722,25 @@
         <v>30</v>
       </c>
       <c r="H51" s="9" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I51" s="35" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J51" s="9" t="n"/>
       <c r="K51" s="35" t="n"/>
       <c r="L51" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M51" s="35" t="n">
         <v>2</v>
-      </c>
-      <c r="M51" s="35" t="n">
-        <v>4</v>
       </c>
       <c r="N51" s="35" t="n"/>
       <c r="O51" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P51" s="3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4285714285714285</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1" s="53">
@@ -11690,7 +11767,9 @@
       <c r="I52" s="35" t="n">
         <v>0</v>
       </c>
-      <c r="J52" s="9" t="n"/>
+      <c r="J52" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K52" s="35" t="n"/>
       <c r="L52" s="35" t="n"/>
       <c r="M52" s="35" t="n">
@@ -11713,31 +11792,31 @@
       <c r="F53" s="166" t="n"/>
       <c r="G53" s="7" t="n"/>
       <c r="H53" s="7" t="n">
-        <v>252</v>
+        <v>201</v>
       </c>
       <c r="I53" s="7" t="n">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="J53" s="7" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K53" s="7" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L53" s="7" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M53" s="7" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="N53" s="7" t="n">
         <v>0</v>
       </c>
       <c r="O53" s="7" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="P53" s="39" t="n">
-        <v>0.7692307692307693</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1" s="53">
@@ -11775,11 +11854,11 @@
         <v>0</v>
       </c>
       <c r="J54" s="9" t="n"/>
-      <c r="K54" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="K54" s="35" t="n"/>
       <c r="L54" s="35" t="n"/>
-      <c r="M54" s="35" t="n"/>
+      <c r="M54" s="35" t="n">
+        <v>1</v>
+      </c>
       <c r="N54" s="35" t="n"/>
       <c r="O54" s="35" t="n"/>
       <c r="P54" s="3" t="n"/>
@@ -11809,11 +11888,11 @@
         <v>0</v>
       </c>
       <c r="J55" s="9" t="n"/>
-      <c r="K55" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="K55" s="35" t="n"/>
       <c r="L55" s="35" t="n"/>
-      <c r="M55" s="35" t="n"/>
+      <c r="M55" s="35" t="n">
+        <v>1</v>
+      </c>
       <c r="N55" s="35" t="n"/>
       <c r="O55" s="35" t="n"/>
       <c r="P55" s="3" t="n"/>
@@ -11845,18 +11924,16 @@
         </is>
       </c>
       <c r="H56" s="9" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I56" s="35" t="n">
         <v>0</v>
       </c>
-      <c r="J56" s="9" t="n">
-        <v>2</v>
-      </c>
+      <c r="J56" s="9" t="n"/>
       <c r="K56" s="35" t="n"/>
       <c r="L56" s="35" t="n"/>
       <c r="M56" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N56" s="35" t="n"/>
       <c r="O56" s="35" t="n"/>
@@ -11880,18 +11957,12 @@
         <v>1</v>
       </c>
       <c r="G57" s="161" t="n"/>
-      <c r="H57" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I57" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H57" s="9" t="n"/>
+      <c r="I57" s="35" t="n"/>
       <c r="J57" s="9" t="n"/>
       <c r="K57" s="35" t="n"/>
       <c r="L57" s="35" t="n"/>
-      <c r="M57" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M57" s="35" t="n"/>
       <c r="N57" s="35" t="n"/>
       <c r="O57" s="35" t="n"/>
       <c r="P57" s="3" t="n"/>
@@ -11923,26 +11994,18 @@
         </is>
       </c>
       <c r="H58" s="9" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I58" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="J58" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="J58" s="9" t="n"/>
       <c r="K58" s="35" t="n"/>
       <c r="L58" s="35" t="n"/>
-      <c r="M58" s="35" t="n">
-        <v>4</v>
-      </c>
+      <c r="M58" s="35" t="n"/>
       <c r="N58" s="35" t="n"/>
-      <c r="O58" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P58" s="3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="O58" s="35" t="n"/>
+      <c r="P58" s="3" t="n"/>
     </row>
     <row r="59" ht="15.75" customHeight="1" s="53">
       <c r="A59" s="192" t="n"/>
@@ -12003,7 +12066,7 @@
         </is>
       </c>
       <c r="H60" s="9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I60" s="35" t="n">
         <v>1</v>
@@ -12012,15 +12075,11 @@
       <c r="K60" s="35" t="n"/>
       <c r="L60" s="35" t="n"/>
       <c r="M60" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N60" s="35" t="n"/>
-      <c r="O60" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P60" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O60" s="35" t="n"/>
+      <c r="P60" s="3" t="n"/>
     </row>
     <row r="61" ht="15.75" customHeight="1" s="53">
       <c r="A61" s="192" t="n"/>
@@ -12077,27 +12136,25 @@
         </is>
       </c>
       <c r="H62" s="9" t="n">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="I62" s="35" t="n">
-        <v>50</v>
-      </c>
-      <c r="J62" s="9" t="n">
-        <v>11</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J62" s="9" t="n"/>
       <c r="K62" s="35" t="n"/>
       <c r="L62" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="M62" s="35" t="n">
         <v>5</v>
-      </c>
-      <c r="M62" s="35" t="n">
-        <v>14</v>
       </c>
       <c r="N62" s="35" t="n"/>
       <c r="O62" s="35" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="P62" s="3" t="n">
-        <v>0.54</v>
+        <v>0.2941176470588235</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1" s="53">
@@ -12119,26 +12176,22 @@
       </c>
       <c r="G63" s="161" t="n"/>
       <c r="H63" s="9" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I63" s="35" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J63" s="9" t="n">
         <v>2</v>
       </c>
       <c r="K63" s="35" t="n"/>
       <c r="L63" s="35" t="n"/>
-      <c r="M63" s="35" t="n"/>
-      <c r="N63" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="O63" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="P63" s="3" t="n">
-        <v>0.3333333333333333</v>
-      </c>
+      <c r="M63" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="N63" s="35" t="n"/>
+      <c r="O63" s="35" t="n"/>
+      <c r="P63" s="3" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="53">
       <c r="A64" s="192" t="n"/>
@@ -12167,27 +12220,27 @@
         </is>
       </c>
       <c r="H64" s="9" t="n">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I64" s="35" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J64" s="9" t="n">
         <v>2</v>
       </c>
       <c r="K64" s="35" t="n"/>
       <c r="L64" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M64" s="35" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N64" s="35" t="n"/>
       <c r="O64" s="35" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="P64" s="3" t="n">
-        <v>0.6904761904761905</v>
+        <v>0.2777777777777778</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1" s="53">
@@ -12311,29 +12364,27 @@
         </is>
       </c>
       <c r="H68" s="9" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I68" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="J68" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="K68" s="35" t="n"/>
+      <c r="L68" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M68" s="35" t="n">
         <v>6</v>
-      </c>
-      <c r="J68" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K68" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="L68" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="M68" s="35" t="n">
-        <v>5</v>
       </c>
       <c r="N68" s="35" t="n"/>
       <c r="O68" s="35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P68" s="3" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1" s="53">
@@ -12358,13 +12409,11 @@
         <v>3</v>
       </c>
       <c r="I69" s="35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J69" s="9" t="n"/>
       <c r="K69" s="35" t="n"/>
-      <c r="L69" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L69" s="35" t="n"/>
       <c r="M69" s="35" t="n"/>
       <c r="N69" s="35" t="n"/>
       <c r="O69" s="35" t="n"/>
@@ -12443,31 +12492,31 @@
       <c r="F72" s="166" t="n"/>
       <c r="G72" s="20" t="n"/>
       <c r="H72" s="20" t="n">
-        <v>194</v>
+        <v>115</v>
       </c>
       <c r="I72" s="20" t="n">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="J72" s="20" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="K72" s="20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L72" s="20" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M72" s="20" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="N72" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O72" s="20" t="n">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="P72" s="39" t="n">
-        <v>0.5945945945945946</v>
+        <v>0.2571428571428571</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="53">
@@ -12495,23 +12544,23 @@
         <v>30</v>
       </c>
       <c r="H73" s="9" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I73" s="35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J73" s="9" t="n"/>
       <c r="K73" s="35" t="n"/>
       <c r="L73" s="35" t="n"/>
       <c r="M73" s="35" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="N73" s="35" t="n"/>
       <c r="O73" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P73" s="3" t="n">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1" s="53">
@@ -12538,23 +12587,21 @@
       <c r="I74" s="35" t="n">
         <v>3</v>
       </c>
-      <c r="J74" s="9" t="n"/>
+      <c r="J74" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K74" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L74" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="L74" s="35" t="n">
-        <v>3</v>
-      </c>
       <c r="M74" s="35" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N74" s="35" t="n"/>
-      <c r="O74" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="P74" s="3" t="n">
-        <v>0.6666666666666666</v>
-      </c>
+      <c r="O74" s="35" t="n"/>
+      <c r="P74" s="3" t="n"/>
     </row>
     <row r="75" ht="15.75" customHeight="1" s="53">
       <c r="A75" s="192" t="n"/>
@@ -12639,10 +12686,10 @@
         <v>30</v>
       </c>
       <c r="H77" s="9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I77" s="35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77" s="9" t="n">
         <v>1</v>
@@ -12650,15 +12697,11 @@
       <c r="K77" s="35" t="n"/>
       <c r="L77" s="35" t="n"/>
       <c r="M77" s="35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N77" s="35" t="n"/>
-      <c r="O77" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P77" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O77" s="35" t="n"/>
+      <c r="P77" s="3" t="n"/>
     </row>
     <row r="78" ht="15.75" customHeight="1" s="53">
       <c r="A78" s="192" t="n"/>
@@ -12679,10 +12722,10 @@
       </c>
       <c r="G78" s="193" t="n"/>
       <c r="H78" s="9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I78" s="35" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J78" s="9" t="n"/>
       <c r="K78" s="35" t="n"/>
@@ -12691,12 +12734,8 @@
         <v>3</v>
       </c>
       <c r="N78" s="35" t="n"/>
-      <c r="O78" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="P78" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O78" s="35" t="n"/>
+      <c r="P78" s="3" t="n"/>
     </row>
     <row r="79" ht="15.75" customHeight="1" s="53">
       <c r="A79" s="192" t="n"/>
@@ -12746,23 +12785,15 @@
         <v>2</v>
       </c>
       <c r="G80" s="161" t="n"/>
-      <c r="H80" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I80" s="35" t="n">
-        <v>4</v>
-      </c>
+      <c r="H80" s="9" t="n"/>
+      <c r="I80" s="35" t="n"/>
       <c r="J80" s="9" t="n"/>
       <c r="K80" s="35" t="n"/>
       <c r="L80" s="35" t="n"/>
       <c r="M80" s="35" t="n"/>
       <c r="N80" s="35" t="n"/>
-      <c r="O80" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="P80" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O80" s="35" t="n"/>
+      <c r="P80" s="3" t="n"/>
     </row>
     <row r="81" ht="15.75" customHeight="1" s="53">
       <c r="A81" s="192" t="n"/>
@@ -12791,15 +12822,15 @@
         </is>
       </c>
       <c r="H81" s="9" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I81" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="J81" s="9" t="n"/>
-      <c r="K81" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="J81" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" s="35" t="n"/>
       <c r="L81" s="35" t="n">
         <v>1</v>
       </c>
@@ -12808,10 +12839,10 @@
       </c>
       <c r="N81" s="35" t="n"/>
       <c r="O81" s="35" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P81" s="3" t="n">
-        <v>0.625</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1" s="53">
@@ -12935,7 +12966,7 @@
         </is>
       </c>
       <c r="H85" s="9" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I85" s="35" t="n">
         <v>3</v>
@@ -12944,18 +12975,16 @@
         <v>1</v>
       </c>
       <c r="K85" s="35" t="n"/>
-      <c r="L85" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L85" s="35" t="n"/>
       <c r="M85" s="35" t="n">
         <v>4</v>
       </c>
       <c r="N85" s="35" t="n"/>
       <c r="O85" s="35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P85" s="3" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1" s="53">
@@ -12976,18 +13005,12 @@
         <v>1</v>
       </c>
       <c r="G86" s="161" t="n"/>
-      <c r="H86" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H86" s="9" t="n"/>
+      <c r="I86" s="35" t="n"/>
       <c r="J86" s="9" t="n"/>
       <c r="K86" s="35" t="n"/>
       <c r="L86" s="35" t="n"/>
-      <c r="M86" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M86" s="35" t="n"/>
       <c r="N86" s="35" t="n"/>
       <c r="O86" s="35" t="n"/>
       <c r="P86" s="3" t="n"/>
@@ -13077,29 +13100,25 @@
         <v>30</v>
       </c>
       <c r="H89" s="9" t="n">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I89" s="35" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="J89" s="9" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K89" s="35" t="n"/>
-      <c r="L89" s="35" t="n">
-        <v>2</v>
-      </c>
+      <c r="L89" s="35" t="n"/>
       <c r="M89" s="35" t="n">
-        <v>10</v>
-      </c>
-      <c r="N89" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="N89" s="35" t="n"/>
       <c r="O89" s="35" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="P89" s="3" t="n">
-        <v>0.8518518518518519</v>
+        <v>0.05263157894736842</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1" s="53">
@@ -13121,24 +13140,22 @@
       </c>
       <c r="G90" s="161" t="n"/>
       <c r="H90" s="9" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I90" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="J90" s="9" t="n"/>
+        <v>1</v>
+      </c>
+      <c r="J90" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K90" s="35" t="n"/>
       <c r="L90" s="35" t="n"/>
       <c r="M90" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N90" s="35" t="n"/>
-      <c r="O90" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P90" s="3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="O90" s="35" t="n"/>
+      <c r="P90" s="3" t="n"/>
     </row>
     <row r="91" ht="15.75" customHeight="1" s="53">
       <c r="A91" s="192" t="n"/>
@@ -13167,27 +13184,23 @@
         </is>
       </c>
       <c r="H91" s="9" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I91" s="35" t="n">
-        <v>14</v>
-      </c>
-      <c r="J91" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="K91" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J91" s="9" t="n"/>
+      <c r="K91" s="35" t="n"/>
       <c r="L91" s="35" t="n"/>
       <c r="M91" s="35" t="n">
         <v>8</v>
       </c>
       <c r="N91" s="35" t="n"/>
       <c r="O91" s="35" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P91" s="3" t="n">
-        <v>0.6428571428571429</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1" s="53">
@@ -13311,7 +13324,7 @@
         </is>
       </c>
       <c r="H95" s="9" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I95" s="35" t="n">
         <v>2</v>
@@ -13319,7 +13332,7 @@
       <c r="J95" s="9" t="n"/>
       <c r="K95" s="35" t="n"/>
       <c r="L95" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M95" s="35" t="n">
         <v>2</v>
@@ -13346,17 +13359,11 @@
         <v>1</v>
       </c>
       <c r="G96" s="161" t="n"/>
-      <c r="H96" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I96" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H96" s="9" t="n"/>
+      <c r="I96" s="35" t="n"/>
       <c r="J96" s="9" t="n"/>
       <c r="K96" s="35" t="n"/>
-      <c r="L96" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L96" s="35" t="n"/>
       <c r="M96" s="35" t="n"/>
       <c r="N96" s="35" t="n"/>
       <c r="O96" s="35" t="n"/>
@@ -13449,30 +13456,20 @@
         </is>
       </c>
       <c r="H99" s="9" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I99" s="35" t="n">
-        <v>12</v>
-      </c>
-      <c r="J99" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K99" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J99" s="9" t="n"/>
+      <c r="K99" s="35" t="n"/>
       <c r="L99" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="M99" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M99" s="35" t="n"/>
       <c r="N99" s="35" t="n"/>
-      <c r="O99" s="35" t="n">
-        <v>7</v>
-      </c>
-      <c r="P99" s="3" t="n">
-        <v>0.5833333333333334</v>
-      </c>
+      <c r="O99" s="35" t="n"/>
+      <c r="P99" s="3" t="n"/>
     </row>
     <row r="100" ht="15.75" customHeight="1" s="53">
       <c r="A100" s="192" t="n"/>
@@ -13581,12 +13578,8 @@
       <c r="L102" s="35" t="n"/>
       <c r="M102" s="35" t="n"/>
       <c r="N102" s="35" t="n"/>
-      <c r="O102" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P102" s="3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="O102" s="35" t="n"/>
+      <c r="P102" s="3" t="n"/>
     </row>
     <row r="103" ht="15.75" customHeight="1" s="53">
       <c r="A103" s="192" t="n"/>
@@ -13755,23 +13748,23 @@
         </is>
       </c>
       <c r="H107" s="9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I107" s="35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J107" s="9" t="n"/>
       <c r="K107" s="35" t="n"/>
       <c r="L107" s="35" t="n"/>
       <c r="M107" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N107" s="35" t="n"/>
       <c r="O107" s="35" t="n">
         <v>3</v>
       </c>
       <c r="P107" s="3" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1" s="53">
@@ -13793,29 +13786,29 @@
       </c>
       <c r="G108" s="161" t="n"/>
       <c r="H108" s="9" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I108" s="35" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J108" s="9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K108" s="35" t="n">
         <v>1</v>
       </c>
       <c r="L108" s="35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M108" s="35" t="n">
         <v>10</v>
       </c>
       <c r="N108" s="35" t="n"/>
       <c r="O108" s="35" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P108" s="3" t="n">
-        <v>0.5</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1" s="53">
@@ -13868,23 +13861,15 @@
         <v>2</v>
       </c>
       <c r="G110" s="161" t="n"/>
-      <c r="H110" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I110" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="H110" s="9" t="n"/>
+      <c r="I110" s="35" t="n"/>
       <c r="J110" s="9" t="n"/>
       <c r="K110" s="35" t="n"/>
       <c r="L110" s="35" t="n"/>
       <c r="M110" s="35" t="n"/>
       <c r="N110" s="35" t="n"/>
-      <c r="O110" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P110" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O110" s="35" t="n"/>
+      <c r="P110" s="3" t="n"/>
     </row>
     <row r="111" ht="15.75" customHeight="1" s="53">
       <c r="A111" s="192" t="n"/>
@@ -13913,22 +13898,18 @@
         </is>
       </c>
       <c r="H111" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I111" s="35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J111" s="9" t="n"/>
       <c r="K111" s="35" t="n"/>
       <c r="L111" s="35" t="n"/>
       <c r="M111" s="35" t="n"/>
       <c r="N111" s="35" t="n"/>
-      <c r="O111" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P111" s="3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="O111" s="35" t="n"/>
+      <c r="P111" s="3" t="n"/>
     </row>
     <row r="112" ht="15.75" customHeight="1" s="53">
       <c r="A112" s="192" t="n"/>
@@ -13991,28 +13972,20 @@
         </is>
       </c>
       <c r="H113" s="9" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I113" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="J113" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="K113" s="35" t="n">
-        <v>2</v>
-      </c>
+      <c r="J113" s="9" t="n"/>
+      <c r="K113" s="35" t="n"/>
       <c r="L113" s="35" t="n"/>
       <c r="M113" s="35" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N113" s="35" t="n"/>
-      <c r="O113" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P113" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O113" s="35" t="n"/>
+      <c r="P113" s="3" t="n"/>
     </row>
     <row r="114" ht="15.75" customHeight="1" s="53">
       <c r="A114" s="192" t="n"/>
@@ -14033,7 +14006,7 @@
       </c>
       <c r="G114" s="161" t="n"/>
       <c r="H114" s="9" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I114" s="35" t="n">
         <v>4</v>
@@ -14042,18 +14015,16 @@
         <v>1</v>
       </c>
       <c r="K114" s="35" t="n"/>
-      <c r="L114" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L114" s="35" t="n"/>
       <c r="M114" s="35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N114" s="35" t="n"/>
       <c r="O114" s="35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P114" s="3" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="115" ht="15.75" customHeight="1" s="53">
@@ -14192,7 +14163,11 @@
           <t>Applied IT Specialist</t>
         </is>
       </c>
-      <c r="D119" s="25" t="n"/>
+      <c r="D119" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>Domestic</t>
@@ -14220,7 +14195,11 @@
       <c r="A120" s="192" t="n"/>
       <c r="B120" s="193" t="n"/>
       <c r="C120" s="161" t="n"/>
-      <c r="D120" s="25" t="n"/>
+      <c r="D120" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E120" s="2" t="inlineStr">
         <is>
           <t>International</t>
@@ -14253,31 +14232,31 @@
       <c r="F121" s="166" t="n"/>
       <c r="G121" s="7" t="n"/>
       <c r="H121" s="7" t="n">
-        <v>278</v>
+        <v>217</v>
       </c>
       <c r="I121" s="7" t="n">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="J121" s="7" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K121" s="7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L121" s="7" t="n">
+        <v>7</v>
+      </c>
+      <c r="M121" s="7" t="n">
+        <v>76</v>
+      </c>
+      <c r="N121" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O121" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="M121" s="7" t="n">
-        <v>83</v>
-      </c>
-      <c r="N121" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O121" s="7" t="n">
-        <v>77</v>
-      </c>
       <c r="P121" s="39" t="n">
-        <v>0.6754385964912281</v>
+        <v>0.2142857142857143</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1" s="53">
@@ -14401,31 +14380,31 @@
       <c r="F125" s="165" t="n"/>
       <c r="G125" s="21" t="n"/>
       <c r="H125" s="22" t="n">
-        <v>724</v>
+        <v>533</v>
       </c>
       <c r="I125" s="22" t="n">
-        <v>342</v>
+        <v>258</v>
       </c>
       <c r="J125" s="22" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K125" s="22" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="L125" s="22" t="n">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="M125" s="22" t="n">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="N125" s="22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O125" s="22" t="n">
-        <v>233</v>
+        <v>76</v>
       </c>
       <c r="P125" s="40" t="n">
-        <v>0.6812865497076024</v>
+        <v>0.2945736434108527</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1" s="53">
@@ -14701,18 +14680,18 @@
       </c>
       <c r="G134" s="36" t="n"/>
       <c r="H134" s="9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I134" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J134" s="9" t="n"/>
+        <v>1</v>
+      </c>
+      <c r="J134" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K134" s="35" t="n">
         <v>1</v>
       </c>
-      <c r="L134" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L134" s="35" t="n"/>
       <c r="M134" s="35" t="n">
         <v>2</v>
       </c>
@@ -14739,10 +14718,10 @@
       </c>
       <c r="G135" s="161" t="n"/>
       <c r="H135" s="9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I135" s="35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J135" s="9" t="n">
         <v>1</v>
@@ -14839,27 +14818,23 @@
       </c>
       <c r="G138" s="35" t="n"/>
       <c r="H138" s="9" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="I138" s="35" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J138" s="9" t="n"/>
-      <c r="K138" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="K138" s="35" t="n"/>
       <c r="L138" s="35" t="n"/>
       <c r="M138" s="35" t="n">
-        <v>13</v>
-      </c>
-      <c r="N138" s="35" t="n">
         <v>8</v>
       </c>
+      <c r="N138" s="35" t="n"/>
       <c r="O138" s="35" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P138" s="3" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="139" ht="15.75" customHeight="1" s="53">
@@ -14881,29 +14856,27 @@
       </c>
       <c r="G139" s="161" t="n"/>
       <c r="H139" s="9" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I139" s="35" t="n">
         <v>20</v>
       </c>
       <c r="J139" s="9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K139" s="35" t="n"/>
       <c r="L139" s="35" t="n">
         <v>2</v>
       </c>
       <c r="M139" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="N139" s="35" t="n">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="N139" s="35" t="n"/>
       <c r="O139" s="35" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P139" s="3" t="n">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="140" ht="15.75" customHeight="1" s="53">
@@ -14933,31 +14906,29 @@
         </is>
       </c>
       <c r="H140" s="9" t="n">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="I140" s="35" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="J140" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K140" s="35" t="n">
+      <c r="K140" s="35" t="n"/>
+      <c r="L140" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="L140" s="35" t="n">
-        <v>3</v>
-      </c>
       <c r="M140" s="35" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="N140" s="35" t="n">
         <v>2</v>
       </c>
       <c r="O140" s="35" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P140" s="3" t="n">
-        <v>1</v>
+        <v>0.6363636363636364</v>
       </c>
     </row>
     <row r="141" ht="15.75" customHeight="1" s="53">
@@ -14979,14 +14950,14 @@
       </c>
       <c r="G141" s="164" t="n"/>
       <c r="H141" s="9" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I141" s="35" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J141" s="9" t="n"/>
       <c r="K141" s="35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L141" s="35" t="n">
         <v>1</v>
@@ -14994,12 +14965,14 @@
       <c r="M141" s="35" t="n">
         <v>8</v>
       </c>
-      <c r="N141" s="35" t="n"/>
+      <c r="N141" s="35" t="n">
+        <v>2</v>
+      </c>
       <c r="O141" s="35" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P141" s="3" t="n">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="142" ht="15.75" customHeight="1" s="53">
@@ -15075,31 +15048,31 @@
       <c r="F144" s="166" t="n"/>
       <c r="G144" s="6" t="n"/>
       <c r="H144" s="7" t="n">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="I144" s="7" t="n">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="J144" s="7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K144" s="7" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="L144" s="7" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M144" s="7" t="n">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="N144" s="7" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="O144" s="7" t="n">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="P144" s="39" t="n">
-        <v>0.75</v>
+        <v>0.4680851063829787</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1" s="53">
@@ -15131,31 +15104,29 @@
         <v>18</v>
       </c>
       <c r="H145" s="9" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I145" s="35" t="n">
         <v>7</v>
       </c>
-      <c r="J145" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="J145" s="9" t="n"/>
       <c r="K145" s="35" t="n">
         <v>1</v>
       </c>
       <c r="L145" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M145" s="35" t="n">
+        <v>9</v>
+      </c>
+      <c r="N145" s="35" t="n">
+        <v>7</v>
+      </c>
+      <c r="O145" s="35" t="n">
         <v>2</v>
       </c>
-      <c r="M145" s="35" t="n">
-        <v>13</v>
-      </c>
-      <c r="N145" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="O145" s="35" t="n">
-        <v>5</v>
-      </c>
       <c r="P145" s="3" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="146" ht="15.75" customHeight="1" s="53">
@@ -15187,19 +15158,19 @@
         <v>1</v>
       </c>
       <c r="L146" s="35" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M146" s="35" t="n">
         <v>3</v>
       </c>
       <c r="N146" s="35" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O146" s="35" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P146" s="3" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.4166666666666667</v>
       </c>
     </row>
     <row r="147" ht="15.75" customHeight="1" s="53">
@@ -15415,31 +15386,27 @@
         <v>30</v>
       </c>
       <c r="H153" s="9" t="n">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="I153" s="35" t="n">
-        <v>21</v>
-      </c>
-      <c r="J153" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K153" s="35" t="n">
-        <v>2</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J153" s="9" t="n"/>
+      <c r="K153" s="35" t="n"/>
       <c r="L153" s="35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M153" s="35" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N153" s="35" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="O153" s="35" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="P153" s="3" t="n">
-        <v>0.7619047619047619</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="154" ht="15.75" customHeight="1" s="53">
@@ -15461,27 +15428,27 @@
       </c>
       <c r="G154" s="197" t="n"/>
       <c r="H154" s="9" t="n">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I154" s="35" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J154" s="9" t="n"/>
       <c r="K154" s="35" t="n"/>
       <c r="L154" s="35" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="M154" s="35" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N154" s="35" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O154" s="35" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P154" s="3" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="155" ht="15.75" customHeight="1" s="53">
@@ -15569,31 +15536,27 @@
         <v>60</v>
       </c>
       <c r="H157" s="9" t="n">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="I157" s="35" t="n">
-        <v>56</v>
-      </c>
-      <c r="J157" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="K157" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="J157" s="9" t="n"/>
+      <c r="K157" s="35" t="n"/>
       <c r="L157" s="35" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M157" s="35" t="n">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="N157" s="35" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="O157" s="35" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="P157" s="3" t="n">
-        <v>0.7678571428571429</v>
+        <v>0.4339622641509434</v>
       </c>
     </row>
     <row r="158" ht="15.75" customHeight="1" s="53">
@@ -15615,29 +15578,27 @@
       </c>
       <c r="G158" s="161" t="n"/>
       <c r="H158" s="9" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I158" s="35" t="n">
-        <v>7</v>
-      </c>
-      <c r="J158" s="9" t="n">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J158" s="9" t="n"/>
       <c r="K158" s="35" t="n"/>
       <c r="L158" s="35" t="n">
         <v>2</v>
       </c>
       <c r="M158" s="35" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N158" s="35" t="n">
         <v>8</v>
       </c>
       <c r="O158" s="35" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P158" s="3" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="159" ht="15.75" customHeight="1" s="53">
@@ -15783,10 +15744,10 @@
       </c>
       <c r="G163" s="35" t="n"/>
       <c r="H163" s="9" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I163" s="35" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J163" s="9" t="n"/>
       <c r="K163" s="35" t="n"/>
@@ -15794,15 +15755,11 @@
         <v>1</v>
       </c>
       <c r="M163" s="35" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="N163" s="35" t="n"/>
-      <c r="O163" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="P163" s="3" t="n">
-        <v>0.75</v>
-      </c>
+      <c r="O163" s="35" t="n"/>
+      <c r="P163" s="3" t="n"/>
     </row>
     <row r="164" ht="15.75" customHeight="1" s="53">
       <c r="A164" s="193" t="n"/>
@@ -15853,31 +15810,31 @@
       <c r="F165" s="166" t="n"/>
       <c r="G165" s="7" t="n"/>
       <c r="H165" s="7" t="n">
-        <v>551</v>
+        <v>488</v>
       </c>
       <c r="I165" s="7" t="n">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="J165" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K165" s="7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L165" s="7" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="M165" s="7" t="n">
-        <v>245</v>
+        <v>223</v>
       </c>
       <c r="N165" s="7" t="n">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="O165" s="7" t="n">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="P165" s="39" t="n">
-        <v>0.7264957264957265</v>
+        <v>0.3761467889908257</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" s="53">
@@ -15893,31 +15850,31 @@
       <c r="F166" s="166" t="n"/>
       <c r="G166" s="5" t="n"/>
       <c r="H166" s="5" t="n">
-        <v>733</v>
+        <v>635</v>
       </c>
       <c r="I166" s="5" t="n">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="J166" s="5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K166" s="5" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="L166" s="5" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="M166" s="5" t="n">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="N166" s="5" t="n">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="O166" s="5" t="n">
-        <v>127</v>
+        <v>63</v>
       </c>
       <c r="P166" s="40" t="n">
-        <v>0.7341040462427746</v>
+        <v>0.4038461538461539</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1" s="53">
@@ -16377,31 +16334,27 @@
         <v>45</v>
       </c>
       <c r="H180" s="9" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I180" s="35" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J180" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="K180" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="L180" s="35" t="n">
-        <v>2</v>
-      </c>
+      <c r="K180" s="35" t="n"/>
+      <c r="L180" s="35" t="n"/>
       <c r="M180" s="35" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="N180" s="35" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O180" s="35" t="n">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="P180" s="3" t="n">
-        <v>0.7321428571428571</v>
+        <v>0.3859649122807017</v>
       </c>
     </row>
     <row r="181" ht="15.75" customHeight="1" s="53">
@@ -16517,27 +16470,23 @@
         <v>45</v>
       </c>
       <c r="H184" s="9" t="n">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I184" s="35" t="n">
-        <v>14</v>
-      </c>
-      <c r="J184" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="K184" s="35" t="n">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J184" s="9" t="n"/>
+      <c r="K184" s="35" t="n"/>
       <c r="L184" s="35" t="n"/>
       <c r="M184" s="35" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="N184" s="35" t="n"/>
       <c r="O184" s="35" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="P184" s="3" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="185" ht="15.75" customHeight="1" s="53">
@@ -16593,26 +16542,22 @@
         <v>20</v>
       </c>
       <c r="H186" s="9" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I186" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="J186" s="9" t="n"/>
+        <v>3</v>
+      </c>
+      <c r="J186" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="K186" s="35" t="n"/>
-      <c r="L186" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L186" s="35" t="n"/>
       <c r="M186" s="35" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N186" s="35" t="n"/>
-      <c r="O186" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P186" s="3" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="O186" s="35" t="n"/>
+      <c r="P186" s="3" t="n"/>
     </row>
     <row r="187" ht="15.75" customHeight="1" s="53">
       <c r="A187" s="193" t="n"/>
@@ -16719,31 +16664,31 @@
       <c r="F190" s="166" t="n"/>
       <c r="G190" s="7" t="n"/>
       <c r="H190" s="4" t="n">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="I190" s="4" t="n">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J190" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K190" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L190" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M190" s="4" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N190" s="4" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O190" s="4" t="n">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="P190" s="39" t="n">
-        <v>0.7407407407407407</v>
+        <v>0.4133333333333333</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" s="53">
@@ -16759,31 +16704,31 @@
       <c r="F191" s="166" t="n"/>
       <c r="G191" s="38" t="n"/>
       <c r="H191" s="5" t="n">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="I191" s="5" t="n">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J191" s="5" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K191" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L191" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M191" s="5" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="N191" s="5" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="O191" s="5" t="n">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="P191" s="40" t="n">
-        <v>0.7407407407407407</v>
+        <v>0.4133333333333333</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" s="53">
@@ -16799,31 +16744,31 @@
       <c r="F192" s="166" t="n"/>
       <c r="G192" s="8" t="n"/>
       <c r="H192" s="8" t="n">
-        <v>1611</v>
+        <v>1297</v>
       </c>
       <c r="I192" s="8" t="n">
-        <v>596</v>
+        <v>489</v>
       </c>
       <c r="J192" s="8" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="K192" s="8" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L192" s="8" t="n">
-        <v>93</v>
+        <v>47</v>
       </c>
       <c r="M192" s="8" t="n">
-        <v>537</v>
+        <v>469</v>
       </c>
       <c r="N192" s="8" t="n">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="O192" s="8" t="n">
-        <v>420</v>
+        <v>170</v>
       </c>
       <c r="P192" s="12" t="n">
-        <v>0.7046979865771812</v>
+        <v>0.3476482617586912</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" s="53">
@@ -17076,7 +17021,29 @@
     <mergeCell ref="C147:C148"/>
     <mergeCell ref="G145:G146"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I120 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I118 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="2">
+      <formula>10</formula>
+      <formula>100000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="1">
+      <formula>1</formula>
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8" dxfId="0">
+      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P118 P121:P1048576">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I119:I120">
     <cfRule type="cellIs" priority="2" operator="between" dxfId="2">
       <formula>10</formula>
       <formula>100000000</formula>
@@ -17086,10 +17053,10 @@
       <formula>9</formula>
     </cfRule>
     <cfRule type="expression" priority="4" dxfId="0">
-      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+      <formula>AND(I119=0, I119&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P119:P120">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
@@ -17111,8 +17078,8 @@
   <dimension ref="A1:P195"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A194" sqref="A194"/>
+      <pane ySplit="2" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G111" sqref="G111:G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -18891,18 +18858,12 @@
         <v>1</v>
       </c>
       <c r="G55" s="161" t="n"/>
-      <c r="H55" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I55" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H55" s="9" t="n"/>
+      <c r="I55" s="35" t="n"/>
       <c r="J55" s="9" t="n"/>
       <c r="K55" s="35" t="n"/>
       <c r="L55" s="35" t="n"/>
-      <c r="M55" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M55" s="35" t="n"/>
       <c r="N55" s="35" t="n"/>
       <c r="O55" s="35" t="n"/>
       <c r="P55" s="3" t="n"/>
@@ -19025,12 +18986,8 @@
         <v>1</v>
       </c>
       <c r="G59" s="161" t="n"/>
-      <c r="H59" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I59" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H59" s="9" t="n"/>
+      <c r="I59" s="35" t="n"/>
       <c r="J59" s="9" t="n"/>
       <c r="K59" s="35" t="n"/>
       <c r="L59" s="35" t="n"/>
@@ -19129,18 +19086,12 @@
           <t>Unlimited</t>
         </is>
       </c>
-      <c r="H62" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="I62" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H62" s="9" t="n"/>
+      <c r="I62" s="35" t="n"/>
       <c r="J62" s="9" t="n"/>
       <c r="K62" s="35" t="n"/>
       <c r="L62" s="35" t="n"/>
-      <c r="M62" s="35" t="n">
-        <v>2</v>
-      </c>
+      <c r="M62" s="35" t="n"/>
       <c r="N62" s="35" t="n"/>
       <c r="O62" s="35" t="n"/>
       <c r="P62" s="3" t="n"/>
@@ -19163,23 +19114,15 @@
         <v>1</v>
       </c>
       <c r="G63" s="161" t="n"/>
-      <c r="H63" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I63" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="H63" s="9" t="n"/>
+      <c r="I63" s="35" t="n"/>
       <c r="J63" s="9" t="n"/>
       <c r="K63" s="35" t="n"/>
       <c r="L63" s="35" t="n"/>
       <c r="M63" s="35" t="n"/>
       <c r="N63" s="35" t="n"/>
-      <c r="O63" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P63" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="O63" s="35" t="n"/>
+      <c r="P63" s="3" t="n"/>
     </row>
     <row r="64" ht="15.75" customHeight="1" s="53">
       <c r="A64" s="192" t="n"/>
@@ -19207,20 +19150,12 @@
           <t>Unlimited</t>
         </is>
       </c>
-      <c r="H64" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I64" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J64" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="H64" s="9" t="n"/>
+      <c r="I64" s="35" t="n"/>
+      <c r="J64" s="9" t="n"/>
       <c r="K64" s="35" t="n"/>
       <c r="L64" s="35" t="n"/>
-      <c r="M64" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M64" s="35" t="n"/>
       <c r="N64" s="35" t="n"/>
       <c r="O64" s="35" t="n"/>
       <c r="P64" s="3" t="n"/>
@@ -19243,18 +19178,12 @@
         <v>1</v>
       </c>
       <c r="G65" s="161" t="n"/>
-      <c r="H65" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I65" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H65" s="9" t="n"/>
+      <c r="I65" s="35" t="n"/>
       <c r="J65" s="9" t="n"/>
       <c r="K65" s="35" t="n"/>
       <c r="L65" s="35" t="n"/>
-      <c r="M65" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M65" s="35" t="n"/>
       <c r="N65" s="35" t="n"/>
       <c r="O65" s="35" t="n"/>
       <c r="P65" s="3" t="n"/>
@@ -19373,18 +19302,12 @@
         <v>1</v>
       </c>
       <c r="G69" s="161" t="n"/>
-      <c r="H69" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I69" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H69" s="9" t="n"/>
+      <c r="I69" s="35" t="n"/>
       <c r="J69" s="9" t="n"/>
       <c r="K69" s="35" t="n"/>
       <c r="L69" s="35" t="n"/>
-      <c r="M69" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M69" s="35" t="n"/>
       <c r="N69" s="35" t="n"/>
       <c r="O69" s="35" t="n"/>
       <c r="P69" s="3" t="n"/>
@@ -19462,13 +19385,13 @@
       <c r="F72" s="166" t="n"/>
       <c r="G72" s="20" t="n"/>
       <c r="H72" s="20" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I72" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K72" s="20" t="n">
         <v>0</v>
@@ -19477,16 +19400,16 @@
         <v>0</v>
       </c>
       <c r="M72" s="20" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N72" s="20" t="n">
         <v>0</v>
       </c>
       <c r="O72" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P72" s="39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1" s="53">
@@ -19907,18 +19830,12 @@
         <v>1</v>
       </c>
       <c r="G86" s="161" t="n"/>
-      <c r="H86" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I86" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H86" s="9" t="n"/>
+      <c r="I86" s="35" t="n"/>
       <c r="J86" s="9" t="n"/>
       <c r="K86" s="35" t="n"/>
       <c r="L86" s="35" t="n"/>
-      <c r="M86" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M86" s="35" t="n"/>
       <c r="N86" s="35" t="n"/>
       <c r="O86" s="35" t="n"/>
       <c r="P86" s="3" t="n"/>
@@ -20099,18 +20016,12 @@
         <v>1</v>
       </c>
       <c r="G92" s="161" t="n"/>
-      <c r="H92" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I92" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H92" s="9" t="n"/>
+      <c r="I92" s="35" t="n"/>
       <c r="J92" s="9" t="n"/>
       <c r="K92" s="35" t="n"/>
       <c r="L92" s="35" t="n"/>
-      <c r="M92" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M92" s="35" t="n"/>
       <c r="N92" s="35" t="n"/>
       <c r="O92" s="35" t="n"/>
       <c r="P92" s="3" t="n"/>
@@ -20230,10 +20141,10 @@
       </c>
       <c r="G96" s="161" t="n"/>
       <c r="H96" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I96" s="35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J96" s="9" t="n"/>
       <c r="K96" s="35" t="n"/>
@@ -20329,18 +20240,12 @@
           <t>Unlimited</t>
         </is>
       </c>
-      <c r="H99" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I99" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H99" s="9" t="n"/>
+      <c r="I99" s="35" t="n"/>
       <c r="J99" s="9" t="n"/>
       <c r="K99" s="35" t="n"/>
       <c r="L99" s="35" t="n"/>
-      <c r="M99" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M99" s="35" t="n"/>
       <c r="N99" s="35" t="n"/>
       <c r="O99" s="35" t="n"/>
       <c r="P99" s="3" t="n"/>
@@ -20775,15 +20680,9 @@
           <t>Unlimited</t>
         </is>
       </c>
-      <c r="H113" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I113" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J113" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="H113" s="9" t="n"/>
+      <c r="I113" s="35" t="n"/>
+      <c r="J113" s="9" t="n"/>
       <c r="K113" s="35" t="n"/>
       <c r="L113" s="35" t="n"/>
       <c r="M113" s="35" t="n"/>
@@ -20809,18 +20708,12 @@
         <v>1</v>
       </c>
       <c r="G114" s="161" t="n"/>
-      <c r="H114" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I114" s="35" t="n">
-        <v>0</v>
-      </c>
+      <c r="H114" s="9" t="n"/>
+      <c r="I114" s="35" t="n"/>
       <c r="J114" s="9" t="n"/>
       <c r="K114" s="35" t="n"/>
       <c r="L114" s="35" t="n"/>
-      <c r="M114" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M114" s="35" t="n"/>
       <c r="N114" s="35" t="n"/>
       <c r="O114" s="35" t="n"/>
       <c r="P114" s="3" t="n"/>
@@ -20961,7 +20854,11 @@
           <t>Applied IT Specialist</t>
         </is>
       </c>
-      <c r="D119" s="25" t="n"/>
+      <c r="D119" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>Domestic</t>
@@ -20975,12 +20872,20 @@
           <t>Unlimited</t>
         </is>
       </c>
-      <c r="H119" s="9" t="n"/>
-      <c r="I119" s="35" t="n"/>
-      <c r="J119" s="9" t="n"/>
+      <c r="H119" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="I119" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J119" s="9" t="n">
+        <v>3</v>
+      </c>
       <c r="K119" s="35" t="n"/>
       <c r="L119" s="35" t="n"/>
-      <c r="M119" s="35" t="n"/>
+      <c r="M119" s="35" t="n">
+        <v>4</v>
+      </c>
       <c r="N119" s="35" t="n"/>
       <c r="O119" s="35" t="n"/>
       <c r="P119" s="3" t="n"/>
@@ -20989,7 +20894,11 @@
       <c r="A120" s="192" t="n"/>
       <c r="B120" s="193" t="n"/>
       <c r="C120" s="161" t="n"/>
-      <c r="D120" s="25" t="n"/>
+      <c r="D120" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E120" s="2" t="inlineStr">
         <is>
           <t>International</t>
@@ -20999,15 +20908,29 @@
         <v>1</v>
       </c>
       <c r="G120" s="161" t="n"/>
-      <c r="H120" s="9" t="n"/>
-      <c r="I120" s="35" t="n"/>
-      <c r="J120" s="9" t="n"/>
+      <c r="H120" s="9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I120" s="35" t="n">
+        <v>5</v>
+      </c>
+      <c r="J120" s="9" t="n">
+        <v>2</v>
+      </c>
       <c r="K120" s="35" t="n"/>
       <c r="L120" s="35" t="n"/>
-      <c r="M120" s="35" t="n"/>
-      <c r="N120" s="35" t="n"/>
-      <c r="O120" s="35" t="n"/>
-      <c r="P120" s="3" t="n"/>
+      <c r="M120" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="N120" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="O120" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P120" s="3" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="121" ht="15.75" customHeight="1" s="53">
       <c r="A121" s="192" t="n"/>
@@ -21022,31 +20945,31 @@
       <c r="F121" s="166" t="n"/>
       <c r="G121" s="7" t="n"/>
       <c r="H121" s="7" t="n">
+        <v>23</v>
+      </c>
+      <c r="I121" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="J121" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="K121" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L121" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="I121" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J121" s="7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K121" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L121" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M121" s="7" t="n">
-        <v>4</v>
-      </c>
       <c r="N121" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O121" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P121" s="39" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="122" ht="15.75" customHeight="1" s="53">
@@ -21170,13 +21093,13 @@
       <c r="F125" s="165" t="n"/>
       <c r="G125" s="21" t="n"/>
       <c r="H125" s="22" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I125" s="22" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J125" s="22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K125" s="22" t="n">
         <v>0</v>
@@ -21185,16 +21108,16 @@
         <v>0</v>
       </c>
       <c r="M125" s="22" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="N125" s="22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O125" s="22" t="n">
         <v>1</v>
       </c>
       <c r="P125" s="40" t="n">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="126" ht="15.75" customHeight="1" s="53">
@@ -21317,20 +21240,12 @@
         <v>1</v>
       </c>
       <c r="G129" s="197" t="n"/>
-      <c r="H129" s="9" t="n">
-        <v>3</v>
-      </c>
-      <c r="I129" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J129" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="H129" s="9" t="n"/>
+      <c r="I129" s="35" t="n"/>
+      <c r="J129" s="9" t="n"/>
       <c r="K129" s="35" t="n"/>
       <c r="L129" s="35" t="n"/>
-      <c r="M129" s="35" t="n">
-        <v>2</v>
-      </c>
+      <c r="M129" s="35" t="n"/>
       <c r="N129" s="35" t="n"/>
       <c r="O129" s="35" t="n"/>
       <c r="P129" s="3" t="n"/>
@@ -21359,22 +21274,12 @@
       <c r="G130" s="204" t="n">
         <v>25</v>
       </c>
-      <c r="H130" s="9" t="n">
-        <v>4</v>
-      </c>
-      <c r="I130" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J130" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="H130" s="9" t="n"/>
+      <c r="I130" s="35" t="n"/>
+      <c r="J130" s="9" t="n"/>
       <c r="K130" s="35" t="n"/>
-      <c r="L130" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="M130" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="L130" s="35" t="n"/>
+      <c r="M130" s="35" t="n"/>
       <c r="N130" s="35" t="n"/>
       <c r="O130" s="35" t="n"/>
       <c r="P130" s="3" t="n"/>
@@ -21397,23 +21302,13 @@
         <v>1</v>
       </c>
       <c r="G131" s="164" t="n"/>
-      <c r="H131" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="I131" s="35" t="n">
-        <v>8</v>
-      </c>
-      <c r="J131" s="9" t="n">
-        <v>3</v>
-      </c>
+      <c r="H131" s="9" t="n"/>
+      <c r="I131" s="35" t="n"/>
+      <c r="J131" s="9" t="n"/>
       <c r="K131" s="35" t="n"/>
       <c r="L131" s="35" t="n"/>
-      <c r="M131" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="N131" s="35" t="n">
-        <v>5</v>
-      </c>
+      <c r="M131" s="35" t="n"/>
+      <c r="N131" s="35" t="n"/>
       <c r="O131" s="35" t="n"/>
       <c r="P131" s="3" t="n"/>
     </row>
@@ -21498,24 +21393,18 @@
       </c>
       <c r="G134" s="36" t="n"/>
       <c r="H134" s="9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I134" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J134" s="9" t="n"/>
       <c r="K134" s="35" t="n"/>
       <c r="L134" s="35" t="n"/>
-      <c r="M134" s="35" t="n">
-        <v>1</v>
-      </c>
+      <c r="M134" s="35" t="n"/>
       <c r="N134" s="35" t="n"/>
-      <c r="O134" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P134" s="3" t="n">
-        <v>0.3333333333333333</v>
-      </c>
+      <c r="O134" s="35" t="n"/>
+      <c r="P134" s="3" t="n"/>
     </row>
     <row r="135" ht="15.75" customHeight="1" s="53">
       <c r="A135" s="193" t="n"/>
@@ -21536,18 +21425,16 @@
       </c>
       <c r="G135" s="161" t="n"/>
       <c r="H135" s="9" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I135" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J135" s="9" t="n"/>
-      <c r="K135" s="35" t="n">
-        <v>6</v>
-      </c>
-      <c r="L135" s="35" t="n">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="J135" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K135" s="35" t="n"/>
+      <c r="L135" s="35" t="n"/>
       <c r="M135" s="35" t="n"/>
       <c r="N135" s="35" t="n"/>
       <c r="O135" s="35" t="n"/>
@@ -21806,31 +21693,31 @@
       <c r="F144" s="166" t="n"/>
       <c r="G144" s="6" t="n"/>
       <c r="H144" s="7" t="n">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="I144" s="7" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="J144" s="7" t="n">
         <v>5</v>
       </c>
       <c r="K144" s="7" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L144" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M144" s="7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N144" s="7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O144" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P144" s="39" t="n">
-        <v>0.07692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" ht="15.75" customHeight="1" s="53">
@@ -21861,20 +21748,12 @@
       <c r="G145" s="206" t="n">
         <v>18</v>
       </c>
-      <c r="H145" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="I145" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="J145" s="9" t="n">
-        <v>1</v>
-      </c>
+      <c r="H145" s="9" t="n"/>
+      <c r="I145" s="35" t="n"/>
+      <c r="J145" s="9" t="n"/>
       <c r="K145" s="35" t="n"/>
       <c r="L145" s="35" t="n"/>
-      <c r="M145" s="35" t="n">
-        <v>3</v>
-      </c>
+      <c r="M145" s="35" t="n"/>
       <c r="N145" s="35" t="n"/>
       <c r="O145" s="35" t="n"/>
       <c r="P145" s="3" t="n"/>
@@ -21897,29 +21776,15 @@
         <v>1</v>
       </c>
       <c r="G146" s="195" t="n"/>
-      <c r="H146" s="9" t="n">
-        <v>20</v>
-      </c>
-      <c r="I146" s="35" t="n">
-        <v>6</v>
-      </c>
-      <c r="J146" s="9" t="n">
-        <v>2</v>
-      </c>
+      <c r="H146" s="9" t="n"/>
+      <c r="I146" s="35" t="n"/>
+      <c r="J146" s="9" t="n"/>
       <c r="K146" s="35" t="n"/>
       <c r="L146" s="35" t="n"/>
-      <c r="M146" s="35" t="n">
-        <v>7</v>
-      </c>
-      <c r="N146" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="O146" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="P146" s="3" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="M146" s="35" t="n"/>
+      <c r="N146" s="35" t="n"/>
+      <c r="O146" s="35" t="n"/>
+      <c r="P146" s="3" t="n"/>
     </row>
     <row r="147" ht="15.75" customHeight="1" s="53">
       <c r="A147" s="193" t="n"/>
@@ -22480,13 +22345,13 @@
       <c r="F165" s="166" t="n"/>
       <c r="G165" s="7" t="n"/>
       <c r="H165" s="7" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I165" s="7" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J165" s="7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K165" s="7" t="n">
         <v>0</v>
@@ -22495,16 +22360,16 @@
         <v>0</v>
       </c>
       <c r="M165" s="7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N165" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O165" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P165" s="39" t="n">
-        <v>0.1428571428571428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" ht="15.75" customHeight="1" s="53">
@@ -22520,31 +22385,31 @@
       <c r="F166" s="166" t="n"/>
       <c r="G166" s="5" t="n"/>
       <c r="H166" s="5" t="n">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="I166" s="5" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J166" s="5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K166" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L166" s="5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M166" s="5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="N166" s="5" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="O166" s="5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P166" s="40" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" ht="15.75" customHeight="1" s="53">
@@ -22995,27 +22860,15 @@
       <c r="G180" s="35" t="n">
         <v>45</v>
       </c>
-      <c r="H180" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="I180" s="35" t="n">
-        <v>12</v>
-      </c>
-      <c r="J180" s="9" t="n">
-        <v>4</v>
-      </c>
+      <c r="H180" s="9" t="n"/>
+      <c r="I180" s="35" t="n"/>
+      <c r="J180" s="9" t="n"/>
       <c r="K180" s="35" t="n"/>
       <c r="L180" s="35" t="n"/>
-      <c r="M180" s="35" t="n">
-        <v>6</v>
-      </c>
+      <c r="M180" s="35" t="n"/>
       <c r="N180" s="35" t="n"/>
-      <c r="O180" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="P180" s="3" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="O180" s="35" t="n"/>
+      <c r="P180" s="3" t="n"/>
     </row>
     <row r="181" ht="15.75" customHeight="1" s="53">
       <c r="A181" s="193" t="n"/>
@@ -23130,7 +22983,7 @@
         <v>45</v>
       </c>
       <c r="H184" s="9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I184" s="35" t="n">
         <v>0</v>
@@ -23139,7 +22992,7 @@
       <c r="K184" s="35" t="n"/>
       <c r="L184" s="35" t="n"/>
       <c r="M184" s="35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N184" s="35" t="n"/>
       <c r="O184" s="35" t="n"/>
@@ -23306,13 +23159,13 @@
       <c r="F190" s="166" t="n"/>
       <c r="G190" s="7" t="n"/>
       <c r="H190" s="4" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="I190" s="4" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J190" s="4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K190" s="4" t="n">
         <v>0</v>
@@ -23321,16 +23174,16 @@
         <v>0</v>
       </c>
       <c r="M190" s="4" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N190" s="4" t="n">
         <v>0</v>
       </c>
       <c r="O190" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P190" s="39" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" ht="15.75" customHeight="1" s="53">
@@ -23346,13 +23199,13 @@
       <c r="F191" s="166" t="n"/>
       <c r="G191" s="38" t="n"/>
       <c r="H191" s="5" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="I191" s="5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J191" s="5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K191" s="5" t="n">
         <v>0</v>
@@ -23361,16 +23214,16 @@
         <v>0</v>
       </c>
       <c r="M191" s="5" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="N191" s="5" t="n">
         <v>0</v>
       </c>
       <c r="O191" s="5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P191" s="40" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" ht="15.75" customHeight="1" s="53">
@@ -23386,31 +23239,31 @@
       <c r="F192" s="166" t="n"/>
       <c r="G192" s="8" t="n"/>
       <c r="H192" s="8" t="n">
-        <v>118</v>
+        <v>33</v>
       </c>
       <c r="I192" s="8" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="J192" s="8" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K192" s="8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L192" s="8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M192" s="8" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="N192" s="8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O192" s="8" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="P192" s="12" t="n">
-        <v>0.1764705882352941</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="193" ht="15.75" customHeight="1" s="53">
@@ -23697,9 +23550,9 @@
   </sheetPr>
   <dimension ref="A1:P195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C200" sqref="C200"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H119" sqref="H119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -25707,10 +25560,10 @@
         </is>
       </c>
       <c r="H62" s="9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I62" s="35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62" s="9" t="n"/>
       <c r="K62" s="35" t="n"/>
@@ -26009,10 +25862,10 @@
       <c r="F72" s="166" t="n"/>
       <c r="G72" s="20" t="n"/>
       <c r="H72" s="20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I72" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" s="20" t="n">
         <v>0</v>
@@ -27474,7 +27327,11 @@
           <t>Applied IT Specialist</t>
         </is>
       </c>
-      <c r="D119" s="25" t="n"/>
+      <c r="D119" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E119" s="2" t="inlineStr">
         <is>
           <t>Domestic</t>
@@ -27502,7 +27359,11 @@
       <c r="A120" s="192" t="n"/>
       <c r="B120" s="193" t="n"/>
       <c r="C120" s="161" t="n"/>
-      <c r="D120" s="25" t="n"/>
+      <c r="D120" s="25" t="inlineStr">
+        <is>
+          <t>AITS</t>
+        </is>
+      </c>
       <c r="E120" s="2" t="inlineStr">
         <is>
           <t>International</t>
@@ -27683,10 +27544,10 @@
       <c r="F125" s="165" t="n"/>
       <c r="G125" s="21" t="n"/>
       <c r="H125" s="22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I125" s="22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J125" s="22" t="n">
         <v>0</v>
@@ -29813,10 +29674,10 @@
       <c r="F192" s="166" t="n"/>
       <c r="G192" s="8" t="n"/>
       <c r="H192" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I192" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J192" s="8" t="n">
         <v>0</v>
@@ -30090,7 +29951,29 @@
     <mergeCell ref="C147:C148"/>
     <mergeCell ref="G145:G146"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I120 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+  <conditionalFormatting sqref="I3:I52 I54:I71 I73:I118 I122:I123 I126:I143 I145:I164 I167:I174 I176:I189">
+    <cfRule type="cellIs" priority="6" operator="between" dxfId="2">
+      <formula>10</formula>
+      <formula>100000000</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="between" dxfId="1">
+      <formula>1</formula>
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="expression" priority="8" dxfId="0">
+      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P118 P121:P1048576">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0.6"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I119:I120">
     <cfRule type="cellIs" priority="2" operator="between" dxfId="2">
       <formula>10</formula>
       <formula>100000000</formula>
@@ -30100,10 +29983,10 @@
       <formula>9</formula>
     </cfRule>
     <cfRule type="expression" priority="4" dxfId="0">
-      <formula>AND(I3=0, I3&lt;&gt;"")</formula>
+      <formula>AND(I119=0, I119&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
+  <conditionalFormatting sqref="P119:P120">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>

</xml_diff>